<commit_message>
Excel config with API-side filter compiles
</commit_message>
<xml_diff>
--- a/tests/001_JustDataSource.xlsx
+++ b/tests/001_JustDataSource.xlsx
@@ -435,9 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>

</xml_diff>